<commit_message>
added US01 & US02 to sprint report
</commit_message>
<xml_diff>
--- a/Team_Parth_Sanket_Vedadnya_Pranav.xlsx
+++ b/Team_Parth_Sanket_Vedadnya_Pranav.xlsx
@@ -5,10 +5,10 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanketpatidar/Desktop/CS 555/Agile Github/CS-555-Agile_Project_Team/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parthxparab/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156DF3E7-114B-9E45-A2C3-96A6B941F633}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5183017-5023-9A47-BA8F-3761E2440FE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15480" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,9 +31,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -44,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="225">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -725,6 +723,30 @@
   </si>
   <si>
     <t>31-35</t>
+  </si>
+  <si>
+    <t>US01()</t>
+  </si>
+  <si>
+    <t>US02()</t>
+  </si>
+  <si>
+    <t>371-401</t>
+  </si>
+  <si>
+    <t>403 - 416</t>
+  </si>
+  <si>
+    <t>test_userstory01()</t>
+  </si>
+  <si>
+    <t>test_userstory02()</t>
+  </si>
+  <si>
+    <t>18-20</t>
+  </si>
+  <si>
+    <t>22-24</t>
   </si>
 </sst>
 </file>
@@ -3109,8 +3131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3198,16 +3220,33 @@
       <c r="F2">
         <v>600</v>
       </c>
+      <c r="G2">
+        <v>27</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>206</v>
+      </c>
       <c r="J2" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
+      <c r="K2" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>219</v>
+      </c>
       <c r="M2" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
+      <c r="N2" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="26" t="s">
@@ -3228,11 +3267,32 @@
       <c r="F3">
         <v>600</v>
       </c>
+      <c r="G3">
+        <v>13</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>206</v>
+      </c>
       <c r="J3" s="17" t="s">
         <v>207</v>
       </c>
+      <c r="K3" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>220</v>
+      </c>
       <c r="M3" s="17" t="s">
         <v>212</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.15">

</xml_diff>